<commit_message>
Add nullable support. Add exceptions on bind fails.
</commit_message>
<xml_diff>
--- a/ExcelBinderTestCore/Documents/Cars.xlsx
+++ b/ExcelBinderTestCore/Documents/Cars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>HP</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>BMW</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Juke</t>
   </si>
 </sst>
 </file>
@@ -381,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,6 +475,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>